<commit_message>
implment importer cell value and its test cases.
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355"/>
   </bookViews>
   <sheets>
     <sheet name="First" sheetId="1" r:id="rId1"/>
     <sheet name="Second" sheetId="2" r:id="rId2"/>
     <sheet name="Third" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>B1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,26 +64,58 @@
   <si>
     <t>H5</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -109,13 +141,22 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -128,7 +169,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -202,7 +243,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -237,7 +277,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,27 +452,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+      <c r="C2">
+        <v>123.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
+        <v>41618</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.61400462962962965</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <f>SUM(10,20)</f>
+        <v>30</v>
+      </c>
+      <c r="C4" t="b">
+        <f>ISBLANK(B1)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" t="str">
+        <f>B1</f>
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="e">
+        <v>#NAME?</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -441,16 +548,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -478,7 +585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="B5" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
refine importing with error type cell
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -456,7 +456,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -523,6 +523,12 @@
       </c>
       <c r="B5" t="e">
         <v>#NAME?</v>
+      </c>
+      <c r="C5" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D5" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* test import API * implement importing cell style and its test cases
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -4,66 +4,74 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="First" sheetId="1" r:id="rId1"/>
-    <sheet name="Second" sheetId="2" r:id="rId2"/>
+    <sheet name="Value" sheetId="1" r:id="rId1"/>
+    <sheet name="Style" sheetId="4" r:id="rId2"/>
     <sheet name="Third" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'[1]sheet-autofilter'!$A$1:$B$8</definedName>
+    <definedName name="RangeMerged">'[1]cell-data'!$F$12</definedName>
+    <definedName name="TestRange1">'[1]cell-data'!$B$12:$D$13</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
   <si>
     <t>B1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>D1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>F1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>H1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>A3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>E3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>G3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>B5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>D5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>F5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>H5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>text</t>
@@ -88,15 +96,220 @@
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <t>font color</t>
+  </si>
+  <si>
+    <t>RGB value</t>
+  </si>
+  <si>
+    <t>ff0000</t>
+  </si>
+  <si>
+    <t>00ff00</t>
+  </si>
+  <si>
+    <t>0000ff</t>
+  </si>
+  <si>
+    <t>Font family</t>
+  </si>
+  <si>
+    <t>arial, arial black, calibri, comic sans ms, courier new, georigia, impact, lucida console, lucida sans unicode, palatino linotype, tahoma, times new roman, trebuchet ms, verdana, ms sans serif, ms serif</t>
+  </si>
+  <si>
+    <t>arial</t>
+  </si>
+  <si>
+    <t>arial black</t>
+  </si>
+  <si>
+    <t>calibri</t>
+  </si>
+  <si>
+    <t>comic sans MS</t>
+  </si>
+  <si>
+    <t>courier new</t>
+  </si>
+  <si>
+    <t>georgia</t>
+  </si>
+  <si>
+    <t>impact</t>
+  </si>
+  <si>
+    <t>lucida console</t>
+  </si>
+  <si>
+    <t>lucida sans unicode</t>
+  </si>
+  <si>
+    <t>palatino linotype</t>
+  </si>
+  <si>
+    <t>tahoma</t>
+  </si>
+  <si>
+    <t>times new roman</t>
+  </si>
+  <si>
+    <t>trebuchet ms</t>
+  </si>
+  <si>
+    <t>verdana</t>
+  </si>
+  <si>
+    <t>ms sans serif</t>
+  </si>
+  <si>
+    <t>ms serif (not exist)</t>
+  </si>
+  <si>
+    <t>book antiqua (ZSS not support)</t>
+  </si>
+  <si>
+    <t>font size</t>
+  </si>
+  <si>
+    <t>boundary case</t>
+  </si>
+  <si>
+    <t>size 8</t>
+  </si>
+  <si>
+    <t>size 12</t>
+  </si>
+  <si>
+    <t>size 28</t>
+  </si>
+  <si>
+    <t>font style</t>
+  </si>
+  <si>
+    <t>bold</t>
+  </si>
+  <si>
+    <t>italic</t>
+  </si>
+  <si>
+    <t>strikethrough</t>
+  </si>
+  <si>
+    <t>underline</t>
+  </si>
+  <si>
+    <t>double underline</t>
+  </si>
+  <si>
+    <t>single accounting</t>
+  </si>
+  <si>
+    <t>double accounting</t>
+  </si>
+  <si>
+    <t>Cell background color</t>
+  </si>
+  <si>
+    <t>Aribitrary Combined</t>
+  </si>
+  <si>
+    <t>georgia,size 12, italic</t>
+  </si>
+  <si>
+    <t>times new roman, size 20,bold</t>
+  </si>
+  <si>
+    <t>0000ff (font), 00ff00 (background)</t>
+  </si>
+  <si>
+    <t>text overflow</t>
+  </si>
+  <si>
+    <t>this a is very very long sentence, and it should be displayed cross multiple columns.</t>
+  </si>
+  <si>
+    <t>block the long sentence</t>
+  </si>
+  <si>
+    <t>text wrapping</t>
+  </si>
+  <si>
+    <t>a very long sentence could be wrapped in multiple lines, if you configure it in "cell properties".</t>
+  </si>
+  <si>
+    <t>a very long sentence with new line.
+A new line starts.
+A second new line starts.</t>
+  </si>
+  <si>
+    <t>vertical alignment</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>middle</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>horizontal alignment</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>combined</t>
+  </si>
+  <si>
+    <t>top left</t>
+  </si>
+  <si>
+    <t>middle center</t>
+  </si>
+  <si>
+    <t>bottom right</t>
+  </si>
+  <si>
+    <t>hyperlink</t>
+  </si>
+  <si>
+    <t>http://www.zkoss.org</t>
+  </si>
+  <si>
+    <t>Type Offset</t>
+  </si>
+  <si>
+    <t>superscript</t>
+  </si>
+  <si>
+    <t>subscript</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
-    <font>
-      <sz val="12"/>
+  <fonts count="53">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -118,13 +331,384 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Comic Sans MS"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Impact"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Microsoft Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Book Antiqua"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="72"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="double"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="doubleAccounting"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,12 +720,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -151,12 +740,155 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -166,6 +898,111 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="cell-text"/>
+      <sheetName val="cell-border"/>
+      <sheetName val="cell-border-unsupported"/>
+      <sheetName val="cell-data"/>
+      <sheetName val="cell-reference"/>
+      <sheetName val="row"/>
+      <sheetName val="column"/>
+      <sheetName val="rowcolumn"/>
+      <sheetName val="chart-image"/>
+      <sheetName val="chart-unsupported"/>
+      <sheetName val="sheet-autofilter"/>
+      <sheetName val="sheet-protection"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="12">
+          <cell r="B12">
+            <v>1</v>
+          </cell>
+          <cell r="C12">
+            <v>2</v>
+          </cell>
+          <cell r="D12">
+            <v>3</v>
+          </cell>
+          <cell r="F12">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>4</v>
+          </cell>
+          <cell r="C13">
+            <v>5</v>
+          </cell>
+          <cell r="D13">
+            <v>6</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>autofilter</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>week day (only Sunday appears)</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>Monday</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Tuesday</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>Wednesday</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>Thursday</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>Friday</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>Saturday</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>Sunday</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="11"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -455,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -532,7 +1369,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -540,16 +1377,385 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.75" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12.625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11" style="5" customWidth="1"/>
+    <col min="8" max="8" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="5" customWidth="1"/>
+    <col min="11" max="11" width="12.25" style="5" customWidth="1"/>
+    <col min="12" max="12" width="9.625" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="21">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:13" ht="51.75">
+      <c r="A4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="12"/>
+    </row>
+    <row r="5" spans="1:13" ht="48.75">
+      <c r="A5" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+    </row>
+    <row r="6" spans="1:13" ht="21">
+      <c r="A6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+    </row>
+    <row r="7" spans="1:13" ht="92.25">
+      <c r="A7" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="29">
+        <v>72</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="35"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75">
+      <c r="A8" s="12"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+    </row>
+    <row r="9" spans="1:13" ht="21">
+      <c r="A9" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="34.5">
+      <c r="A10" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="21">
+      <c r="A11" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="21">
+      <c r="A13" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="127.5">
+      <c r="B14" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="1:13" ht="128.25">
+      <c r="A15" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="128.25">
+      <c r="A16" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.75">
+      <c r="A19" s="54"/>
+      <c r="B19" s="54"/>
+    </row>
+    <row r="20" spans="1:4" ht="21">
+      <c r="A20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="55"/>
+    </row>
+    <row r="21" spans="1:4" ht="18.75">
+      <c r="A21" s="54"/>
+      <c r="B21" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+    </row>
+    <row r="22" spans="1:4" ht="20.25">
+      <c r="A22" s="54"/>
+      <c r="B22" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="55"/>
+    </row>
+    <row r="23" spans="1:4" ht="18.75">
+      <c r="A23" s="54"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+    </row>
+    <row r="24" spans="1:4" ht="21">
+      <c r="A24" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="55"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+    </row>
+    <row r="25" spans="1:4" ht="76.5">
+      <c r="A25" s="4"/>
+      <c r="B25" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+    </row>
+    <row r="26" spans="1:4" ht="60">
+      <c r="B26" s="57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A27" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="60" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="21">
+      <c r="A28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="63" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="49.5" customHeight="1">
+      <c r="A29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="63" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="21">
+      <c r="A31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="66" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="27" customHeight="1">
+      <c r="A33" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="69" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="70" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B6:J6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B31" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -606,7 +1812,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* update class header and author * impoert row style
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
   <si>
     <t>B1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -321,6 +321,18 @@
   </si>
   <si>
     <t>2013.4.12</t>
+  </si>
+  <si>
+    <t>font with color #0000FF</t>
+  </si>
+  <si>
+    <t>size 14</t>
+  </si>
+  <si>
+    <t>Row Style 1</t>
+  </si>
+  <si>
+    <t>Row Style 2</t>
   </si>
 </sst>
 </file>
@@ -333,7 +345,7 @@
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
   </numFmts>
-  <fonts count="54">
+  <fonts count="56">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -721,6 +733,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -772,7 +800,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -922,10 +950,6 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -945,6 +969,12 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -953,6 +983,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1381,10 +1416,10 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="71">
+      <c r="B2" s="69">
         <v>123</v>
       </c>
-      <c r="C2" s="72">
+      <c r="C2" s="70">
         <v>123.45</v>
       </c>
     </row>
@@ -1439,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1485,17 +1520,17 @@
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
@@ -1567,17 +1602,17 @@
       <c r="A6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
     </row>
     <row r="7" spans="1:13" ht="92.25">
       <c r="A7" s="26" t="s">
@@ -1806,6 +1841,28 @@
       </c>
       <c r="C33" s="68" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="86" customFormat="1" ht="15.75">
+      <c r="A35" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="86" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="86" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="87" customFormat="1" ht="18.75">
+      <c r="A36" s="87" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="87" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1883,7 +1940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1899,82 +1956,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="72" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="75"/>
-      <c r="B2" s="76">
+      <c r="A2" s="73"/>
+      <c r="B2" s="74">
         <v>1234.56</v>
       </c>
-      <c r="C2" s="77">
+      <c r="C2" s="75">
         <v>1234.56</v>
       </c>
-      <c r="D2" s="78">
+      <c r="D2" s="76">
         <v>1234</v>
       </c>
-      <c r="E2" s="79">
+      <c r="E2" s="77">
         <v>41376</v>
       </c>
-      <c r="F2" s="80">
+      <c r="F2" s="78">
         <v>0.7583333333333333</v>
       </c>
-      <c r="G2" s="81">
+      <c r="G2" s="79">
         <v>0.123</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="75"/>
-      <c r="B3" s="74" t="s">
+      <c r="A3" s="73"/>
+      <c r="B3" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="74" t="s">
+      <c r="E3" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="75"/>
-      <c r="B4" s="82">
+      <c r="A4" s="73"/>
+      <c r="B4" s="80">
         <v>0.48</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="81">
         <v>1000000000</v>
       </c>
-      <c r="D4" s="84" t="s">
+      <c r="D4" s="82" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="85">
+      <c r="E4" s="83">
         <v>73504450</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
import - cell - wrap test, locked, alignment
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -4,16 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="1" r:id="rId1"/>
     <sheet name="Style" sheetId="4" r:id="rId2"/>
     <sheet name="Third" sheetId="3" r:id="rId3"/>
-    <sheet name="Format" sheetId="5" r:id="rId4"/>
+    <sheet name="column" sheetId="7" r:id="rId4"/>
+    <sheet name="Format" sheetId="5" r:id="rId5"/>
+    <sheet name="sheet-protection" sheetId="6" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'[1]sheet-autofilter'!$A$1:$B$8</definedName>
@@ -25,54 +27,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="102">
   <si>
     <t>B1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>D1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>F1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>H1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>A3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>C3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>E3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>G3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>B5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>D5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>F5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>H5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>text</t>
@@ -333,6 +335,18 @@
   </si>
   <si>
     <t>Row Style 2</t>
+  </si>
+  <si>
+    <t>This sheet is protected and cannot be edited.</t>
+  </si>
+  <si>
+    <t>This cell is editable.</t>
+  </si>
+  <si>
+    <t>The first column is freezed.</t>
+  </si>
+  <si>
+    <t>the column E is hiding.</t>
   </si>
 </sst>
 </file>
@@ -345,9 +359,25 @@
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
   </numFmts>
-  <fonts count="56">
-    <font>
-      <sz val="12"/>
+  <fonts count="58">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -790,17 +820,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -810,154 +842,154 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -969,17 +1001,25 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 4" xfId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1466,7 +1506,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1476,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1520,17 +1560,17 @@
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
@@ -1602,17 +1642,17 @@
       <c r="A6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:13" ht="92.25">
       <c r="A7" s="26" t="s">
@@ -1843,25 +1883,25 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="86" customFormat="1" ht="15.75">
-      <c r="A35" s="86" t="s">
+    <row r="35" spans="1:3" s="84" customFormat="1" ht="15.75">
+      <c r="A35" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="86" t="s">
+      <c r="B35" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="86" t="s">
+      <c r="C35" s="84" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="87" customFormat="1" ht="18.75">
-      <c r="A36" s="87" t="s">
+    <row r="36" spans="1:3" s="85" customFormat="1" ht="18.75">
+      <c r="A36" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="B36" s="87" t="s">
+      <c r="B36" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="87" t="s">
+      <c r="C36" s="85" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1931,12 +1971,42 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22" style="91" customWidth="1"/>
+    <col min="2" max="4" width="9" style="91"/>
+    <col min="5" max="5" width="0" style="91" hidden="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="91"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="91" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -2036,4 +2106,41 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.375" style="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="86"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="90" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
import cell filled color
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="1" r:id="rId1"/>
@@ -1007,12 +1007,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1516,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1560,17 +1560,17 @@
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
@@ -1642,17 +1642,17 @@
       <c r="A6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="89"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="89"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
     </row>
     <row r="7" spans="1:13" ht="92.25">
       <c r="A7" s="26" t="s">
@@ -1980,24 +1980,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22" style="91" customWidth="1"/>
-    <col min="2" max="4" width="9" style="91"/>
-    <col min="5" max="5" width="0" style="91" hidden="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="91"/>
+    <col min="1" max="1" width="22" style="88" customWidth="1"/>
+    <col min="2" max="4" width="9" style="88"/>
+    <col min="5" max="5" width="0" style="88" hidden="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="88"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="88" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="88" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2123,13 +2123,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="87" t="s">

</xml_diff>

<commit_message>
* import fill pattern * import column & row hidden
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Value" sheetId="1" r:id="rId1"/>
     <sheet name="Style" sheetId="4" r:id="rId2"/>
     <sheet name="Third" sheetId="3" r:id="rId3"/>
-    <sheet name="column" sheetId="7" r:id="rId4"/>
+    <sheet name="column-row" sheetId="7" r:id="rId4"/>
     <sheet name="cell-border" sheetId="8" r:id="rId5"/>
     <sheet name="Format" sheetId="5" r:id="rId6"/>
     <sheet name="sheet-protection" sheetId="6" r:id="rId7"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="133">
   <si>
     <t>B1</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -432,6 +432,15 @@
   </si>
   <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>Fill pattern</t>
+  </si>
+  <si>
+    <t>solid</t>
+  </si>
+  <si>
+    <t>The row 10 - 15 is hidden</t>
   </si>
 </sst>
 </file>
@@ -894,7 +903,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -917,6 +926,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0000FF"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="65"/>
+        <bgColor theme="3" tint="0.39991454817346722"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkGray">
+        <fgColor theme="3" tint="0.39994506668294322"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -1225,7 +1246,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1432,6 +1453,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1951,10 +1974,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1997,17 +2020,17 @@
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="120" t="s">
+      <c r="B3" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
@@ -2079,17 +2102,17 @@
       <c r="A6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="123" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="121"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="121"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="123"/>
     </row>
     <row r="7" spans="1:13" ht="92.25">
       <c r="A7" s="26" t="s">
@@ -2341,6 +2364,15 @@
       <c r="C36" s="85" t="s">
         <v>95</v>
       </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" s="120" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2415,11 +2447,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F5" sqref="F5"/>
+      <selection pane="topRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2455,6 +2487,17 @@
       </c>
       <c r="F3" s="119"/>
     </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="118" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1"/>
+    <row r="11" spans="1:6" hidden="1"/>
+    <row r="12" spans="1:6" hidden="1"/>
+    <row r="13" spans="1:6" hidden="1"/>
+    <row r="14" spans="1:6" hidden="1"/>
+    <row r="15" spans="1:6" hidden="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2700,34 +2743,34 @@
       <c r="A28" s="89" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="122" t="s">
+      <c r="B28" s="124" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="123"/>
-      <c r="E28" s="122" t="s">
+      <c r="C28" s="125"/>
+      <c r="E28" s="124" t="s">
         <v>124</v>
       </c>
-      <c r="F28" s="124"/>
-      <c r="G28" s="123"/>
+      <c r="F28" s="126"/>
+      <c r="G28" s="125"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="125" t="s">
+      <c r="B31" s="127" t="s">
         <v>125</v>
       </c>
-      <c r="C31" s="128" t="s">
+      <c r="C31" s="130" t="s">
         <v>126</v>
       </c>
-      <c r="D31" s="129"/>
+      <c r="D31" s="131"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="126"/>
-      <c r="C32" s="130"/>
-      <c r="D32" s="131"/>
+      <c r="B32" s="128"/>
+      <c r="C32" s="132"/>
+      <c r="D32" s="133"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="127"/>
-      <c r="C33" s="132"/>
-      <c r="D33" s="133"/>
+      <c r="B33" s="129"/>
+      <c r="C33" s="134"/>
+      <c r="D33" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2857,13 +2900,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="136" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="87" t="s">

</xml_diff>

<commit_message>
* test a column having empty cells and changed width * pull up converting methods * isolate a method to get XSSF font color
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -2451,7 +2451,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9"/>
+      <selection pane="topRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2461,7 +2461,9 @@
     <col min="3" max="3" width="12.75" style="88" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="88" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="0" style="88" hidden="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="88"/>
+    <col min="6" max="13" width="9" style="88"/>
+    <col min="14" max="14" width="10" style="88" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="88"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
* import freeze, grid line display * add HSSFSheetHelper temporarily to get freeze information
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="1" r:id="rId1"/>
@@ -2449,9 +2449,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2510,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
* import named range * import sheet protection
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="15075" windowHeight="5355" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="1" r:id="rId1"/>
     <sheet name="Style" sheetId="4" r:id="rId2"/>
-    <sheet name="Third" sheetId="3" r:id="rId3"/>
+    <sheet name="NamedRange" sheetId="3" r:id="rId3"/>
     <sheet name="column-row" sheetId="7" r:id="rId4"/>
     <sheet name="cell-border" sheetId="8" r:id="rId5"/>
     <sheet name="Format" sheetId="5" r:id="rId6"/>
@@ -20,63 +20,15 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'[1]sheet-autofilter'!$A$1:$B$8</definedName>
-    <definedName name="RangeMerged">'[1]cell-data'!$F$12</definedName>
-    <definedName name="TestRange1">'[1]cell-data'!$B$12:$D$13</definedName>
+    <definedName name="RangeMerged">NamedRange!$F$2</definedName>
+    <definedName name="TestRange1">NamedRange!$B$2:$D$3</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="133">
-  <si>
-    <t>B1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>D1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>F1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>H1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>A3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>C3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>E3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>G3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>B5</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>D5</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>F5</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>H5</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="124">
   <si>
     <t>text</t>
   </si>
@@ -441,6 +393,15 @@
   </si>
   <si>
     <t>The row 10 - 15 is hidden</t>
+  </si>
+  <si>
+    <t>named range</t>
+  </si>
+  <si>
+    <t>TestRange1</t>
+  </si>
+  <si>
+    <t>RangeMerged</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1207,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1472,6 +1433,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1514,42 +1488,22 @@
       <sheetName val="sheet-protection"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3">
         <row r="12">
           <cell r="B12">
             <v>1</v>
           </cell>
-          <cell r="C12">
-            <v>2</v>
-          </cell>
-          <cell r="D12">
-            <v>3</v>
-          </cell>
-          <cell r="F12">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>4</v>
-          </cell>
-          <cell r="C13">
-            <v>5</v>
-          </cell>
-          <cell r="D13">
-            <v>6</v>
-          </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
       <sheetData sheetId="10">
         <row r="1">
           <cell r="A1" t="str">
@@ -1595,7 +1549,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="11"/>
+      <sheetData sheetId="11" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1900,21 +1854,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B2" s="69">
         <v>123</v>
@@ -1925,7 +1879,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>41618</v>
@@ -1936,7 +1890,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <f>SUM(10,20)</f>
@@ -1953,7 +1907,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" t="e">
         <v>#NAME?</v>
@@ -1999,29 +1953,29 @@
   <sheetData>
     <row r="1" spans="1:13" ht="21">
       <c r="A1" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="6" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="31.5" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B3" s="122" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C3" s="122"/>
       <c r="D3" s="122"/>
@@ -2037,58 +1991,58 @@
     </row>
     <row r="4" spans="1:13" ht="51.75">
       <c r="A4" s="10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="K4" s="20" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:13" ht="48.75">
       <c r="A5" s="21" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -2100,10 +2054,10 @@
     </row>
     <row r="6" spans="1:13" ht="21">
       <c r="A6" s="4" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B6" s="123" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C6" s="123"/>
       <c r="D6" s="123"/>
@@ -2116,13 +2070,13 @@
     </row>
     <row r="7" spans="1:13" ht="92.25">
       <c r="A7" s="26" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D7" s="29">
         <v>72</v>
@@ -2149,82 +2103,82 @@
     </row>
     <row r="9" spans="1:13" ht="21">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="34.5">
       <c r="A10" s="36" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="F10" s="41" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="21">
       <c r="A11" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="43" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="21">
       <c r="A13" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="127.5">
       <c r="B14" s="46" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C14" s="47" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:13" ht="128.25">
       <c r="A15" s="48" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="128.25">
       <c r="A16" s="51" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18.75">
@@ -2233,14 +2187,14 @@
     </row>
     <row r="20" spans="1:4" ht="21">
       <c r="A20" s="4" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D20" s="55"/>
     </row>
     <row r="21" spans="1:4" ht="18.75">
       <c r="A21" s="54"/>
       <c r="B21" s="55" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C21" s="55"/>
       <c r="D21" s="55"/>
@@ -2248,10 +2202,10 @@
     <row r="22" spans="1:4" ht="20.25">
       <c r="A22" s="54"/>
       <c r="B22" s="55" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C22" s="56" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D22" s="55"/>
     </row>
@@ -2263,7 +2217,7 @@
     </row>
     <row r="24" spans="1:4" ht="21">
       <c r="A24" s="4" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B24" s="55"/>
       <c r="C24" s="55"/>
@@ -2272,105 +2226,105 @@
     <row r="25" spans="1:4" ht="76.5">
       <c r="A25" s="4"/>
       <c r="B25" s="57" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C25" s="55"/>
       <c r="D25" s="55"/>
     </row>
     <row r="26" spans="1:4" ht="60">
       <c r="B26" s="57" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="48.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B27" s="58" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C27" s="59" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D27" s="60" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="21">
       <c r="A28" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B28" s="61" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C28" s="62" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D28" s="63" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="49.5" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B29" s="64" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C29" s="65" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D29" s="63" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="21">
       <c r="A31" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B31" s="66" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="27" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B33" s="67" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C33" s="68" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="84" customFormat="1" ht="15.75">
       <c r="A35" s="84" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B35" s="84" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C35" s="84" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="85" customFormat="1" ht="18.75">
       <c r="A36" s="85" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B36" s="85" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C36" s="85" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="5" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B38" s="120" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C38" s="121"/>
     </row>
@@ -2389,57 +2343,95 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="1" spans="1:8" ht="21">
+      <c r="A1" s="71" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="72" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="73">
+        <f>SUM(TestRange1)</f>
+        <v>21</v>
+      </c>
+      <c r="D1" s="137"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="73">
+        <f>SUM(RangeMerged,F4:H4)</f>
+        <v>10</v>
+      </c>
+      <c r="H1" s="73"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="73"/>
+      <c r="B2" s="138">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C2" s="139">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="D2" s="140">
         <v>3</v>
       </c>
+      <c r="E2" s="73"/>
+      <c r="F2" s="141">
+        <v>1</v>
+      </c>
+      <c r="G2" s="142"/>
+      <c r="H2" s="143"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="s">
+      <c r="A3" s="73"/>
+      <c r="B3" s="144">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="145">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" s="146">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
+      <c r="E3" s="73"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="148"/>
+      <c r="H3" s="149"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="73"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73">
+        <v>2</v>
+      </c>
+      <c r="G4" s="73">
+        <v>3</v>
+      </c>
+      <c r="H4" s="73">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:H3"/>
+  </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2470,30 +2462,30 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="118" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D1" s="88" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F1" s="119" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="118" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="F2" s="119"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="118" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="F3" s="119"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="118" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:6" hidden="1"/>
@@ -2512,7 +2504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2533,16 +2525,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21">
       <c r="A1" s="89" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B1" s="90" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C1" s="91" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D1" s="92" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21">
@@ -2553,59 +2545,59 @@
     </row>
     <row r="3" spans="1:7" ht="21">
       <c r="A3" s="89" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B3" s="95" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C3" s="96" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D3" s="97" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="E3" s="98" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" s="99" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D5" s="101" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" s="102" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C9" s="102" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E9" s="103" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="F9" s="104" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" s="102" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C10" s="102" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="E10" s="105"/>
       <c r="F10" s="106"/>
     </row>
     <row r="12" spans="1:7">
       <c r="B12" s="106" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C12" s="105"/>
       <c r="G12" s="94"/>
@@ -2622,13 +2614,13 @@
     </row>
     <row r="15" spans="1:7">
       <c r="B15" s="107" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C15" s="108"/>
     </row>
     <row r="16" spans="1:7">
       <c r="B16" s="109" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C16" s="110"/>
     </row>
@@ -2646,25 +2638,25 @@
     </row>
     <row r="19" spans="1:8" ht="15.75">
       <c r="A19" s="111" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B19" s="103" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C19" s="96" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="D19" s="104" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="F19" s="106" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G19" s="112" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="H19" s="105" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2685,84 +2677,84 @@
     </row>
     <row r="23" spans="1:8">
       <c r="B23" s="116" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C23" s="116" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="116" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="117" t="s">
         <v>109</v>
       </c>
-      <c r="D23" s="116" t="s">
-        <v>117</v>
-      </c>
-      <c r="F23" s="117" t="s">
-        <v>121</v>
-      </c>
       <c r="G23" s="117" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="H23" s="117" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="B24" s="116" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C24" s="116" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="116" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="117" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="116" t="s">
-        <v>117</v>
-      </c>
-      <c r="F24" s="117" t="s">
-        <v>121</v>
-      </c>
       <c r="G24" s="117" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="H24" s="117" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" s="116" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C25" s="116" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="116" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" s="117" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="116" t="s">
-        <v>117</v>
-      </c>
-      <c r="F25" s="117" t="s">
-        <v>121</v>
-      </c>
       <c r="G25" s="117" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="H25" s="117" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="21">
       <c r="A28" s="89" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B28" s="124" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C28" s="125"/>
       <c r="E28" s="124" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="F28" s="126"/>
       <c r="G28" s="125"/>
     </row>
     <row r="31" spans="1:8">
       <c r="B31" s="127" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C31" s="130" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D31" s="131"/>
     </row>
@@ -2792,7 +2784,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2808,25 +2800,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21">
       <c r="A1" s="71" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1" s="72" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E1" s="72" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F1" s="72" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="G1" s="72" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2853,16 +2845,16 @@
     <row r="3" spans="1:7">
       <c r="A3" s="73"/>
       <c r="B3" s="72" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D3" s="72" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="F3" s="73"/>
       <c r="G3" s="73"/>
@@ -2876,7 +2868,7 @@
         <v>1000000000</v>
       </c>
       <c r="D4" s="82" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E4" s="83">
         <v>73504450</v>
@@ -2905,7 +2897,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="136" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B1" s="136"/>
       <c r="C1" s="136"/>
@@ -2914,7 +2906,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="87" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Export Validation. * add XLSX implementation * add more tests on validation type
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="139">
   <si>
     <t>The first column is freezed.</t>
   </si>
@@ -449,6 +449,12 @@
 List
 Warning
 not show dropdown</t>
+  </si>
+  <si>
+    <t>any value validation</t>
+  </si>
+  <si>
+    <t>any value</t>
   </si>
 </sst>
 </file>
@@ -3615,10 +3621,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3627,6 +3633,14 @@
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="131" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" t="s">
+        <v>138</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" ht="46.5">
       <c r="A2" s="135" t="s">
         <v>133</v>

</xml_diff>

<commit_message>
* add custom validation test cases * import all CellRangeAddress
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="142">
   <si>
     <t>The first column is freezed.</t>
   </si>
@@ -455,6 +455,16 @@
   </si>
   <si>
     <t>any value</t>
+  </si>
+  <si>
+    <t>must be text</t>
+  </si>
+  <si>
+    <t>custom validation
+istext()</t>
+  </si>
+  <si>
+    <t>percetage</t>
   </si>
 </sst>
 </file>
@@ -3621,10 +3631,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3633,11 +3643,11 @@
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="23.25">
       <c r="A1" s="131" t="s">
         <v>137</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="136" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3689,17 +3699,39 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45">
+    <row r="6" spans="1:6" ht="46.5">
       <c r="A6" s="135" t="s">
         <v>135</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="136" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="31.5">
+      <c r="A7" s="135" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="136" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="23.25">
+      <c r="A8" s="135" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="136">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="5">
+  <dataValidations count="7">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sorry" error="1 - 10" promptTitle="Notice" prompt="valid between 1 to 10" sqref="B2">
       <formula1>1</formula1>
       <formula2>10</formula2>
@@ -3716,6 +3748,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>"red, blue, green"</formula1>
     </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+      <formula1>ISTEXT(B7)</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+      <formula1>C8</formula1>
+      <formula2>D8</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Import & Export Hyperlink/RichText
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12975" activeTab="7"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="2" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <definedName name="RangeMerged">NamedRange!$F$2</definedName>
     <definedName name="TestRange1">NamedRange!$B$2:$D$3</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="145">
   <si>
     <t>The first column is freezed.</t>
   </si>
@@ -466,22 +466,90 @@
   <si>
     <t>percetage</t>
   </si>
+  <si>
+    <t>rich text</t>
+    <phoneticPr fontId="57" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>abc</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>123</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFC78548"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>xyz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Hello</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF33FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>World</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCC99"/>
+        <rFont val="HGPSoeiKakupoptai"/>
+        <family val="5"/>
+        <charset val="128"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;NT$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_-[$¥-411]* #,##0.00_-;\-[$¥-411]* #,##0.00_-;_-[$¥-411]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
+    <numFmt numFmtId="176" formatCode="&quot;NT$&quot;#,##0.00"/>
+    <numFmt numFmtId="177" formatCode="_-[$¥-411]* #,##0.00_-;\-[$¥-411]* #,##0.00_-;_-[$¥-411]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="0.0%"/>
+    <numFmt numFmtId="179" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
   </numFmts>
-  <fonts count="57">
+  <fonts count="65" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -489,7 +557,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -498,14 +566,14 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -514,7 +582,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -522,14 +590,14 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF00FF00"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -537,7 +605,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -557,7 +625,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -643,7 +711,7 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -651,7 +719,7 @@
     <font>
       <sz val="28"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -659,7 +727,7 @@
     <font>
       <sz val="72"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -667,7 +735,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -675,7 +743,7 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -683,7 +751,7 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -691,7 +759,7 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -699,7 +767,7 @@
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -707,7 +775,7 @@
     <font>
       <sz val="24"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -716,7 +784,7 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -724,7 +792,7 @@
       <strike/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -732,7 +800,7 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -740,7 +808,7 @@
       <u val="double"/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -749,7 +817,7 @@
       <u val="singleAccounting"/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -758,7 +826,7 @@
       <u val="doubleAccounting"/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -820,14 +888,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -849,7 +917,7 @@
       <vertAlign val="superscript"/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -858,7 +926,7 @@
       <vertAlign val="subscript"/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -866,7 +934,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -875,7 +943,7 @@
       <i/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -883,16 +951,71 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFC78548"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF33FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCCCC99"/>
+      <name val="HGPSoeiKakupoptai"/>
+      <family val="5"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1236,7 +1359,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1441,15 +1564,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="4" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="13" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1487,14 +1610,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="4" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="4" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="5"/>
     <cellStyle name="Normal 4" xfId="1"/>
     <cellStyle name="Normal 5" xfId="4"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="3" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1503,11 +1627,16 @@
       <color rgb="FF0000FF"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1581,6 +1710,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1615,6 +1745,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1790,19 +1921,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75">
+    <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1816,7 +1947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -1828,7 +1959,7 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -1840,7 +1971,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1857,7 +1988,7 @@
         <v>B1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
+    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1872,19 +2003,21 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="57" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J3"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -1897,7 +2030,7 @@
     <col min="9" max="9" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
@@ -1916,7 +2049,7 @@
       <c r="L1" s="11"/>
       <c r="M1" s="11"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>15</v>
       </c>
@@ -1939,7 +2072,7 @@
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="1:13" ht="35.25" customHeight="1">
+    <row r="3" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
@@ -1958,7 +2091,7 @@
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
     </row>
-    <row r="4" spans="1:13" ht="36.75">
+    <row r="4" spans="1:13" ht="36.75" x14ac:dyDescent="0.4">
       <c r="A4" s="16" t="s">
         <v>20</v>
       </c>
@@ -1995,7 +2128,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:13" ht="64.5">
+    <row r="5" spans="1:13" ht="64.5" x14ac:dyDescent="0.35">
       <c r="A5" s="27" t="s">
         <v>31</v>
       </c>
@@ -2022,7 +2155,7 @@
       <c r="L5" s="18"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:13" ht="21">
+    <row r="6" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>37</v>
       </c>
@@ -2041,7 +2174,7 @@
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" ht="92.25">
+    <row r="7" spans="1:13" ht="100.5" x14ac:dyDescent="1.45">
       <c r="A7" s="32" t="s">
         <v>39</v>
       </c>
@@ -2064,7 +2197,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75">
+    <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="33"/>
       <c r="C8" s="18"/>
@@ -2079,7 +2212,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="21">
+    <row r="9" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>42</v>
       </c>
@@ -2096,7 +2229,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" ht="34.5">
+    <row r="10" spans="1:13" ht="36" x14ac:dyDescent="0.4">
       <c r="A10" s="42" t="s">
         <v>43</v>
       </c>
@@ -2125,7 +2258,7 @@
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="21">
+    <row r="11" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>50</v>
       </c>
@@ -2142,7 +2275,7 @@
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
         <v>15</v>
       </c>
@@ -2163,7 +2296,7 @@
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="1:13" ht="21">
+    <row r="13" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>51</v>
       </c>
@@ -2180,7 +2313,7 @@
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="1:13" ht="127.5">
+    <row r="14" spans="1:13" ht="127.5" x14ac:dyDescent="0.35">
       <c r="A14" s="11"/>
       <c r="B14" s="52" t="s">
         <v>52</v>
@@ -2199,7 +2332,7 @@
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
     </row>
-    <row r="15" spans="1:13" ht="128.25">
+    <row r="15" spans="1:13" ht="128.25" x14ac:dyDescent="0.4">
       <c r="A15" s="54" t="s">
         <v>15</v>
       </c>
@@ -2220,7 +2353,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:13" ht="128.25">
+    <row r="16" spans="1:13" ht="128.25" x14ac:dyDescent="0.4">
       <c r="A16" s="57" t="s">
         <v>54</v>
       </c>
@@ -2241,7 +2374,7 @@
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -2256,7 +2389,7 @@
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -2271,7 +2404,7 @@
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
     </row>
-    <row r="19" spans="1:13" ht="18.75">
+    <row r="19" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A19" s="60"/>
       <c r="B19" s="60"/>
       <c r="C19" s="11"/>
@@ -2286,7 +2419,7 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" ht="21">
+    <row r="20" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>55</v>
       </c>
@@ -2303,7 +2436,7 @@
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
     </row>
-    <row r="21" spans="1:13" ht="18.75">
+    <row r="21" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A21" s="60"/>
       <c r="B21" s="61" t="s">
         <v>56</v>
@@ -2320,7 +2453,7 @@
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
     </row>
-    <row r="22" spans="1:13" ht="20.25">
+    <row r="22" spans="1:13" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="60"/>
       <c r="B22" s="61" t="s">
         <v>56</v>
@@ -2339,7 +2472,7 @@
       <c r="L22" s="11"/>
       <c r="M22" s="11"/>
     </row>
-    <row r="23" spans="1:13" ht="18.75">
+    <row r="23" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A23" s="60"/>
       <c r="B23" s="61"/>
       <c r="C23" s="61"/>
@@ -2354,7 +2487,7 @@
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
     </row>
-    <row r="24" spans="1:13" ht="21">
+    <row r="24" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>58</v>
       </c>
@@ -2371,7 +2504,7 @@
       <c r="L24" s="11"/>
       <c r="M24" s="11"/>
     </row>
-    <row r="25" spans="1:13" ht="76.5">
+    <row r="25" spans="1:13" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="63" t="s">
         <v>59</v>
@@ -2388,7 +2521,7 @@
       <c r="L25" s="11"/>
       <c r="M25" s="11"/>
     </row>
-    <row r="26" spans="1:13" ht="75">
+    <row r="26" spans="1:13" ht="63" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="63" t="s">
         <v>60</v>
@@ -2405,7 +2538,7 @@
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
     </row>
-    <row r="27" spans="1:13" ht="21">
+    <row r="27" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>61</v>
       </c>
@@ -2428,7 +2561,7 @@
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
     </row>
-    <row r="28" spans="1:13" ht="21">
+    <row r="28" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>65</v>
       </c>
@@ -2451,7 +2584,7 @@
       <c r="L28" s="11"/>
       <c r="M28" s="11"/>
     </row>
-    <row r="29" spans="1:13" ht="21">
+    <row r="29" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>69</v>
       </c>
@@ -2474,7 +2607,7 @@
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -2489,7 +2622,7 @@
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
     </row>
-    <row r="31" spans="1:13" ht="21">
+    <row r="31" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>73</v>
       </c>
@@ -2508,7 +2641,7 @@
       <c r="L31" s="11"/>
       <c r="M31" s="11"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -2523,7 +2656,7 @@
       <c r="L32" s="11"/>
       <c r="M32" s="11"/>
     </row>
-    <row r="33" spans="1:13" ht="21.75">
+    <row r="33" spans="1:13" ht="24" x14ac:dyDescent="0.4">
       <c r="A33" s="10" t="s">
         <v>75</v>
       </c>
@@ -2544,7 +2677,7 @@
       <c r="L33" s="11"/>
       <c r="M33" s="11"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -2559,7 +2692,7 @@
       <c r="L34" s="11"/>
       <c r="M34" s="11"/>
     </row>
-    <row r="35" spans="1:13" s="132" customFormat="1" ht="15.75">
+    <row r="35" spans="1:13" s="132" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="75" t="s">
         <v>78</v>
       </c>
@@ -2580,7 +2713,7 @@
       <c r="L35" s="75"/>
       <c r="M35" s="75"/>
     </row>
-    <row r="36" spans="1:13" s="133" customFormat="1" ht="18.75">
+    <row r="36" spans="1:13" s="133" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A36" s="76" t="s">
         <v>80</v>
       </c>
@@ -2601,7 +2734,7 @@
       <c r="L36" s="76"/>
       <c r="M36" s="76"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -2616,7 +2749,7 @@
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>82</v>
       </c>
@@ -2635,11 +2768,23 @@
       <c r="L38" s="11"/>
       <c r="M38" s="11"/>
     </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" s="160" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="160" t="s">
+        <v>144</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="B6:J6"/>
   </mergeCells>
+  <phoneticPr fontId="57" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B31" r:id="rId1"/>
   </hyperlinks>
@@ -2648,21 +2793,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="79" t="s">
         <v>84</v>
       </c>
@@ -2684,7 +2829,7 @@
       </c>
       <c r="H1" s="81"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="81"/>
       <c r="B2" s="83">
         <v>1</v>
@@ -2702,7 +2847,7 @@
       <c r="G2" s="142"/>
       <c r="H2" s="143"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="81"/>
       <c r="B3" s="86">
         <v>4</v>
@@ -2718,7 +2863,7 @@
       <c r="G3" s="145"/>
       <c r="H3" s="146"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="81"/>
       <c r="B4" s="81"/>
       <c r="C4" s="81"/>
@@ -2738,12 +2883,13 @@
   <mergeCells count="1">
     <mergeCell ref="F2:H3"/>
   </mergeCells>
+  <phoneticPr fontId="57" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2753,7 +2899,7 @@
       <selection pane="bottomRight" activeCell="B13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" style="131" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
@@ -2762,7 +2908,7 @@
     <col min="14" max="14" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75">
+    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2782,7 +2928,7 @@
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="18.75">
+    <row r="2" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2797,7 +2943,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="18.75">
+    <row r="3" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2812,7 +2958,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="18.75">
+    <row r="4" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2825,7 +2971,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="18.75">
+    <row r="5" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2838,7 +2984,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="18.75">
+    <row r="6" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2851,7 +2997,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="18.75">
+    <row r="7" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2864,7 +3010,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="18.75">
+    <row r="8" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2877,7 +3023,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="18.75">
+    <row r="9" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>124</v>
       </c>
@@ -2892,22 +3038,23 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" hidden="1"/>
-    <row r="11" spans="1:11" hidden="1"/>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="57" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
@@ -2915,7 +3062,7 @@
     <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="90" t="s">
         <v>88</v>
       </c>
@@ -2937,7 +3084,7 @@
       <c r="K1" s="94"/>
       <c r="L1" s="94"/>
     </row>
-    <row r="2" spans="1:12" ht="21">
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.3">
       <c r="A2" s="90"/>
       <c r="B2" s="95"/>
       <c r="C2" s="95"/>
@@ -2951,7 +3098,7 @@
       <c r="K2" s="94"/>
       <c r="L2" s="94"/>
     </row>
-    <row r="3" spans="1:12" ht="21">
+    <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.3">
       <c r="A3" s="90" t="s">
         <v>89</v>
       </c>
@@ -2975,7 +3122,7 @@
       <c r="K3" s="94"/>
       <c r="L3" s="94"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="94"/>
       <c r="B4" s="94"/>
       <c r="C4" s="94"/>
@@ -2989,7 +3136,7 @@
       <c r="K4" s="94"/>
       <c r="L4" s="94"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="94"/>
       <c r="B5" s="100" t="s">
         <v>91</v>
@@ -3009,7 +3156,7 @@
       <c r="K5" s="94"/>
       <c r="L5" s="94"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="94"/>
       <c r="B6" s="94"/>
       <c r="C6" s="94"/>
@@ -3023,7 +3170,7 @@
       <c r="K6" s="94"/>
       <c r="L6" s="94"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="94"/>
       <c r="B7" s="94"/>
       <c r="C7" s="94"/>
@@ -3037,7 +3184,7 @@
       <c r="K7" s="94"/>
       <c r="L7" s="94"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="94"/>
       <c r="B8" s="94"/>
       <c r="C8" s="94"/>
@@ -3051,7 +3198,7 @@
       <c r="K8" s="94"/>
       <c r="L8" s="94"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="94"/>
       <c r="B9" s="103" t="s">
         <v>94</v>
@@ -3073,7 +3220,7 @@
       <c r="K9" s="94"/>
       <c r="L9" s="94"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
       <c r="B10" s="103" t="s">
         <v>97</v>
@@ -3091,7 +3238,7 @@
       <c r="K10" s="94"/>
       <c r="L10" s="94"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="94"/>
       <c r="B11" s="94"/>
       <c r="C11" s="94"/>
@@ -3105,7 +3252,7 @@
       <c r="K11" s="94"/>
       <c r="L11" s="94"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="94"/>
       <c r="B12" s="107" t="s">
         <v>99</v>
@@ -3121,7 +3268,7 @@
       <c r="K12" s="94"/>
       <c r="L12" s="94"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="94"/>
       <c r="B13" s="105"/>
       <c r="C13" s="104"/>
@@ -3135,7 +3282,7 @@
       <c r="K13" s="94"/>
       <c r="L13" s="94"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="94"/>
       <c r="B14" s="95"/>
       <c r="C14" s="95"/>
@@ -3149,7 +3296,7 @@
       <c r="K14" s="94"/>
       <c r="L14" s="94"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="94"/>
       <c r="B15" s="108" t="s">
         <v>100</v>
@@ -3165,7 +3312,7 @@
       <c r="K15" s="94"/>
       <c r="L15" s="94"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="94"/>
       <c r="B16" s="110" t="s">
         <v>101</v>
@@ -3181,7 +3328,7 @@
       <c r="K16" s="94"/>
       <c r="L16" s="94"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="94"/>
       <c r="B17" s="95"/>
       <c r="C17" s="95"/>
@@ -3195,7 +3342,7 @@
       <c r="K17" s="94"/>
       <c r="L17" s="94"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="94"/>
       <c r="B18" s="95"/>
       <c r="C18" s="95"/>
@@ -3209,7 +3356,7 @@
       <c r="K18" s="94"/>
       <c r="L18" s="94"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="112" t="s">
         <v>102</v>
       </c>
@@ -3237,7 +3384,7 @@
       <c r="K19" s="94"/>
       <c r="L19" s="94"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="94"/>
       <c r="B20" s="98"/>
       <c r="C20" s="95"/>
@@ -3251,7 +3398,7 @@
       <c r="K20" s="94"/>
       <c r="L20" s="94"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="94"/>
       <c r="B21" s="106"/>
       <c r="C21" s="96"/>
@@ -3265,7 +3412,7 @@
       <c r="K21" s="94"/>
       <c r="L21" s="94"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="94"/>
       <c r="B22" s="94"/>
       <c r="C22" s="94"/>
@@ -3279,7 +3426,7 @@
       <c r="K22" s="94"/>
       <c r="L22" s="94"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="94"/>
       <c r="B23" s="117" t="s">
         <v>106</v>
@@ -3305,7 +3452,7 @@
       <c r="K23" s="94"/>
       <c r="L23" s="94"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="94"/>
       <c r="B24" s="117" t="s">
         <v>106</v>
@@ -3331,7 +3478,7 @@
       <c r="K24" s="94"/>
       <c r="L24" s="94"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="94"/>
       <c r="B25" s="117" t="s">
         <v>106</v>
@@ -3357,7 +3504,7 @@
       <c r="K25" s="94"/>
       <c r="L25" s="94"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="94"/>
       <c r="B26" s="94"/>
       <c r="C26" s="94"/>
@@ -3371,7 +3518,7 @@
       <c r="K26" s="94"/>
       <c r="L26" s="94"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="94"/>
       <c r="B27" s="94"/>
       <c r="C27" s="94"/>
@@ -3385,7 +3532,7 @@
       <c r="K27" s="94"/>
       <c r="L27" s="94"/>
     </row>
-    <row r="28" spans="1:12" ht="21">
+    <row r="28" spans="1:12" ht="21" x14ac:dyDescent="0.3">
       <c r="A28" s="90" t="s">
         <v>108</v>
       </c>
@@ -3405,7 +3552,7 @@
       <c r="K28" s="94"/>
       <c r="L28" s="94"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="94"/>
       <c r="B29" s="94"/>
       <c r="C29" s="94"/>
@@ -3419,7 +3566,7 @@
       <c r="K29" s="94"/>
       <c r="L29" s="94"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="94"/>
       <c r="B30" s="94"/>
       <c r="C30" s="94"/>
@@ -3433,7 +3580,7 @@
       <c r="K30" s="94"/>
       <c r="L30" s="94"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="94"/>
       <c r="B31" s="150" t="s">
         <v>111</v>
@@ -3451,7 +3598,7 @@
       <c r="K31" s="94"/>
       <c r="L31" s="94"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="94"/>
       <c r="B32" s="151"/>
       <c r="C32" s="155"/>
@@ -3465,7 +3612,7 @@
       <c r="K32" s="94"/>
       <c r="L32" s="94"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="94"/>
       <c r="B33" s="152"/>
       <c r="C33" s="157"/>
@@ -3486,19 +3633,20 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="C31:D33"/>
   </mergeCells>
+  <phoneticPr fontId="57" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -3508,7 +3656,7 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="79" t="s">
         <v>113</v>
       </c>
@@ -3531,7 +3679,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="81"/>
       <c r="B2" s="119">
         <v>1234.56</v>
@@ -3552,7 +3700,7 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="81"/>
       <c r="B3" s="80" t="s">
         <v>118</v>
@@ -3569,7 +3717,7 @@
       <c r="F3" s="81"/>
       <c r="G3" s="81"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="81"/>
       <c r="B4" s="125">
         <v>0.48</v>
@@ -3587,21 +3735,22 @@
       <c r="G4" s="81"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="57" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="159" t="s">
         <v>122</v>
       </c>
@@ -3610,7 +3759,7 @@
       <c r="D1" s="159"/>
       <c r="E1" s="159"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="129" t="s">
         <v>123</v>
       </c>
@@ -3624,26 +3773,27 @@
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
+  <phoneticPr fontId="57" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25">
+    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.4">
       <c r="A1" s="131" t="s">
         <v>137</v>
       </c>
@@ -3651,7 +3801,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="46.5">
+    <row r="2" spans="1:6" ht="49.5" x14ac:dyDescent="0.4">
       <c r="A2" s="135" t="s">
         <v>133</v>
       </c>
@@ -3659,7 +3809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="61.5">
+    <row r="3" spans="1:6" ht="65.25" x14ac:dyDescent="0.4">
       <c r="A3" s="135" t="s">
         <v>136</v>
       </c>
@@ -3679,7 +3829,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="46.5">
+    <row r="4" spans="1:6" ht="49.5" x14ac:dyDescent="0.4">
       <c r="A4" s="135" t="s">
         <v>131</v>
       </c>
@@ -3691,7 +3841,7 @@
         <v>41640</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="46.5">
+    <row r="5" spans="1:6" ht="65.25" x14ac:dyDescent="0.4">
       <c r="A5" s="135" t="s">
         <v>134</v>
       </c>
@@ -3699,7 +3849,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="46.5">
+    <row r="6" spans="1:6" ht="49.5" x14ac:dyDescent="0.4">
       <c r="A6" s="135" t="s">
         <v>135</v>
       </c>
@@ -3707,7 +3857,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5">
+    <row r="7" spans="1:6" ht="33.75" x14ac:dyDescent="0.4">
       <c r="A7" s="135" t="s">
         <v>140</v>
       </c>
@@ -3715,7 +3865,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="23.25">
+    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.4">
       <c r="A8" s="135" t="s">
         <v>141</v>
       </c>
@@ -3731,6 +3881,7 @@
     </row>
   </sheetData>
   <dataConsolidate/>
+  <phoneticPr fontId="57" type="noConversion"/>
   <dataValidations count="7">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sorry" error="1 - 10" promptTitle="Notice" prompt="valid between 1 to 10" sqref="B2">
       <formula1>1</formula1>

</xml_diff>

<commit_message>
revert back into origin test case file
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/import.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12975" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12975" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="2" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <definedName name="RangeMerged">NamedRange!$F$2</definedName>
     <definedName name="TestRange1">NamedRange!$B$2:$D$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="142">
   <si>
     <t>The first column is freezed.</t>
   </si>
@@ -466,90 +466,22 @@
   <si>
     <t>percetage</t>
   </si>
-  <si>
-    <t>rich text</t>
-    <phoneticPr fontId="57" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>abc</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>123</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFC78548"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>xyz</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Hello</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF33FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>World</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCC99"/>
-        <rFont val="HGPSoeiKakupoptai"/>
-        <family val="5"/>
-        <charset val="128"/>
-      </rPr>
-      <t>000</t>
-    </r>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="&quot;NT$&quot;#,##0.00"/>
-    <numFmt numFmtId="177" formatCode="_-[$¥-411]* #,##0.00_-;\-[$¥-411]* #,##0.00_-;_-[$¥-411]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="0.0%"/>
-    <numFmt numFmtId="179" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
+    <numFmt numFmtId="164" formatCode="&quot;NT$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-[$¥-411]* #,##0.00_-;\-[$¥-411]* #,##0.00_-;_-[$¥-411]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
   </numFmts>
-  <fonts count="65" x14ac:knownFonts="1">
+  <fonts count="57">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -557,7 +489,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -566,14 +498,14 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF0000FF"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -582,7 +514,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -590,14 +522,14 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF00FF00"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -605,7 +537,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -625,7 +557,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -711,7 +643,7 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -719,7 +651,7 @@
     <font>
       <sz val="28"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -727,7 +659,7 @@
     <font>
       <sz val="72"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -735,7 +667,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -743,7 +675,7 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -751,7 +683,7 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -759,7 +691,7 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -767,7 +699,7 @@
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -775,7 +707,7 @@
     <font>
       <sz val="24"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -784,7 +716,7 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -792,7 +724,7 @@
       <strike/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -800,7 +732,7 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -808,7 +740,7 @@
       <u val="double"/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -817,7 +749,7 @@
       <u val="singleAccounting"/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -826,7 +758,7 @@
       <u val="doubleAccounting"/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -888,14 +820,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -917,7 +849,7 @@
       <vertAlign val="superscript"/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -926,7 +858,7 @@
       <vertAlign val="subscript"/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -934,7 +866,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -943,7 +875,7 @@
       <i/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -951,71 +883,16 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FFC78548"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF33FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCCCC99"/>
-      <name val="HGPSoeiKakupoptai"/>
-      <family val="5"/>
-      <charset val="128"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1359,7 +1236,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1564,15 +1441,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="4" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="13" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1610,15 +1487,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="4" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="4" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="5"/>
     <cellStyle name="Normal 4" xfId="1"/>
     <cellStyle name="Normal 5" xfId="4"/>
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="3" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1627,16 +1503,11 @@
       <color rgb="FF0000FF"/>
     </mruColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1710,7 +1581,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1745,7 +1615,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1921,19 +1790,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1947,7 +1816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -1959,7 +1828,7 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -1971,7 +1840,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1988,7 +1857,7 @@
         <v>B1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -2003,21 +1872,19 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="57" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -2030,7 +1897,7 @@
     <col min="9" max="9" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="21">
       <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
@@ -2049,7 +1916,7 @@
       <c r="L1" s="11"/>
       <c r="M1" s="11"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="12" t="s">
         <v>15</v>
       </c>
@@ -2072,7 +1939,7 @@
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="35.25" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
@@ -2091,7 +1958,7 @@
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
     </row>
-    <row r="4" spans="1:13" ht="36.75" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" ht="36.75">
       <c r="A4" s="16" t="s">
         <v>20</v>
       </c>
@@ -2128,7 +1995,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:13" ht="64.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="64.5">
       <c r="A5" s="27" t="s">
         <v>31</v>
       </c>
@@ -2155,7 +2022,7 @@
       <c r="L5" s="18"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:13" ht="21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="21">
       <c r="A6" s="10" t="s">
         <v>37</v>
       </c>
@@ -2174,7 +2041,7 @@
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" ht="100.5" x14ac:dyDescent="1.45">
+    <row r="7" spans="1:13" ht="92.25">
       <c r="A7" s="32" t="s">
         <v>39</v>
       </c>
@@ -2197,7 +2064,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15.75">
       <c r="A8" s="18"/>
       <c r="B8" s="33"/>
       <c r="C8" s="18"/>
@@ -2212,7 +2079,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="21">
       <c r="A9" s="10" t="s">
         <v>42</v>
       </c>
@@ -2229,7 +2096,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" ht="36" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="34.5">
       <c r="A10" s="42" t="s">
         <v>43</v>
       </c>
@@ -2258,7 +2125,7 @@
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="21">
       <c r="A11" s="10" t="s">
         <v>50</v>
       </c>
@@ -2275,7 +2142,7 @@
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="49" t="s">
         <v>15</v>
       </c>
@@ -2296,7 +2163,7 @@
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="1:13" ht="21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="21">
       <c r="A13" s="10" t="s">
         <v>51</v>
       </c>
@@ -2313,7 +2180,7 @@
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="1:13" ht="127.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="127.5">
       <c r="A14" s="11"/>
       <c r="B14" s="52" t="s">
         <v>52</v>
@@ -2332,7 +2199,7 @@
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
     </row>
-    <row r="15" spans="1:13" ht="128.25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="128.25">
       <c r="A15" s="54" t="s">
         <v>15</v>
       </c>
@@ -2353,7 +2220,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:13" ht="128.25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" ht="128.25">
       <c r="A16" s="57" t="s">
         <v>54</v>
       </c>
@@ -2374,7 +2241,7 @@
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -2389,7 +2256,7 @@
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -2404,7 +2271,7 @@
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
     </row>
-    <row r="19" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="18.75">
       <c r="A19" s="60"/>
       <c r="B19" s="60"/>
       <c r="C19" s="11"/>
@@ -2419,7 +2286,7 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" ht="21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="21">
       <c r="A20" s="10" t="s">
         <v>55</v>
       </c>
@@ -2436,7 +2303,7 @@
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
     </row>
-    <row r="21" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="18.75">
       <c r="A21" s="60"/>
       <c r="B21" s="61" t="s">
         <v>56</v>
@@ -2453,7 +2320,7 @@
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
     </row>
-    <row r="22" spans="1:13" ht="21" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:13" ht="20.25">
       <c r="A22" s="60"/>
       <c r="B22" s="61" t="s">
         <v>56</v>
@@ -2472,7 +2339,7 @@
       <c r="L22" s="11"/>
       <c r="M22" s="11"/>
     </row>
-    <row r="23" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="18.75">
       <c r="A23" s="60"/>
       <c r="B23" s="61"/>
       <c r="C23" s="61"/>
@@ -2487,7 +2354,7 @@
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
     </row>
-    <row r="24" spans="1:13" ht="21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="21">
       <c r="A24" s="10" t="s">
         <v>58</v>
       </c>
@@ -2504,7 +2371,7 @@
       <c r="L24" s="11"/>
       <c r="M24" s="11"/>
     </row>
-    <row r="25" spans="1:13" ht="63.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="76.5">
       <c r="A25" s="10"/>
       <c r="B25" s="63" t="s">
         <v>59</v>
@@ -2521,7 +2388,7 @@
       <c r="L25" s="11"/>
       <c r="M25" s="11"/>
     </row>
-    <row r="26" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="75">
       <c r="A26" s="11"/>
       <c r="B26" s="63" t="s">
         <v>60</v>
@@ -2538,7 +2405,7 @@
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
     </row>
-    <row r="27" spans="1:13" ht="21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="21">
       <c r="A27" s="10" t="s">
         <v>61</v>
       </c>
@@ -2561,7 +2428,7 @@
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
     </row>
-    <row r="28" spans="1:13" ht="21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="21">
       <c r="A28" s="10" t="s">
         <v>65</v>
       </c>
@@ -2584,7 +2451,7 @@
       <c r="L28" s="11"/>
       <c r="M28" s="11"/>
     </row>
-    <row r="29" spans="1:13" ht="21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="21">
       <c r="A29" s="10" t="s">
         <v>69</v>
       </c>
@@ -2607,7 +2474,7 @@
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -2622,7 +2489,7 @@
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
     </row>
-    <row r="31" spans="1:13" ht="21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="21">
       <c r="A31" s="10" t="s">
         <v>73</v>
       </c>
@@ -2641,7 +2508,7 @@
       <c r="L31" s="11"/>
       <c r="M31" s="11"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -2656,7 +2523,7 @@
       <c r="L32" s="11"/>
       <c r="M32" s="11"/>
     </row>
-    <row r="33" spans="1:13" ht="24" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:13" ht="21.75">
       <c r="A33" s="10" t="s">
         <v>75</v>
       </c>
@@ -2677,7 +2544,7 @@
       <c r="L33" s="11"/>
       <c r="M33" s="11"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -2692,7 +2559,7 @@
       <c r="L34" s="11"/>
       <c r="M34" s="11"/>
     </row>
-    <row r="35" spans="1:13" s="132" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="132" customFormat="1" ht="15.75">
       <c r="A35" s="75" t="s">
         <v>78</v>
       </c>
@@ -2713,7 +2580,7 @@
       <c r="L35" s="75"/>
       <c r="M35" s="75"/>
     </row>
-    <row r="36" spans="1:13" s="133" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" s="133" customFormat="1" ht="18.75">
       <c r="A36" s="76" t="s">
         <v>80</v>
       </c>
@@ -2734,7 +2601,7 @@
       <c r="L36" s="76"/>
       <c r="M36" s="76"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -2749,7 +2616,7 @@
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" s="11" t="s">
         <v>82</v>
       </c>
@@ -2768,23 +2635,11 @@
       <c r="L38" s="11"/>
       <c r="M38" s="11"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>142</v>
-      </c>
-      <c r="B40" s="160" t="s">
-        <v>143</v>
-      </c>
-      <c r="C40" s="160" t="s">
-        <v>144</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="B6:J6"/>
   </mergeCells>
-  <phoneticPr fontId="57" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B31" r:id="rId1"/>
   </hyperlinks>
@@ -2793,21 +2648,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="21">
       <c r="A1" s="79" t="s">
         <v>84</v>
       </c>
@@ -2829,7 +2684,7 @@
       </c>
       <c r="H1" s="81"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="81"/>
       <c r="B2" s="83">
         <v>1</v>
@@ -2847,7 +2702,7 @@
       <c r="G2" s="142"/>
       <c r="H2" s="143"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="81"/>
       <c r="B3" s="86">
         <v>4</v>
@@ -2863,7 +2718,7 @@
       <c r="G3" s="145"/>
       <c r="H3" s="146"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="81"/>
       <c r="B4" s="81"/>
       <c r="C4" s="81"/>
@@ -2883,13 +2738,12 @@
   <mergeCells count="1">
     <mergeCell ref="F2:H3"/>
   </mergeCells>
-  <phoneticPr fontId="57" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2899,7 +2753,7 @@
       <selection pane="bottomRight" activeCell="B13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.5703125" style="131" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
@@ -2908,7 +2762,7 @@
     <col min="14" max="14" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2928,7 +2782,7 @@
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2943,7 +2797,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2958,7 +2812,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="18.75">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2971,7 +2825,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="18.75">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2984,7 +2838,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="18.75">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2997,7 +2851,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="18.75">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3010,7 +2864,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="18.75">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3023,7 +2877,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>124</v>
       </c>
@@ -3038,23 +2892,22 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:11" hidden="1"/>
+    <row r="11" spans="1:11" hidden="1"/>
   </sheetData>
-  <phoneticPr fontId="57" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
@@ -3062,7 +2915,7 @@
     <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="21">
       <c r="A1" s="90" t="s">
         <v>88</v>
       </c>
@@ -3084,7 +2937,7 @@
       <c r="K1" s="94"/>
       <c r="L1" s="94"/>
     </row>
-    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="21">
       <c r="A2" s="90"/>
       <c r="B2" s="95"/>
       <c r="C2" s="95"/>
@@ -3098,7 +2951,7 @@
       <c r="K2" s="94"/>
       <c r="L2" s="94"/>
     </row>
-    <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="21">
       <c r="A3" s="90" t="s">
         <v>89</v>
       </c>
@@ -3122,7 +2975,7 @@
       <c r="K3" s="94"/>
       <c r="L3" s="94"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="94"/>
       <c r="B4" s="94"/>
       <c r="C4" s="94"/>
@@ -3136,7 +2989,7 @@
       <c r="K4" s="94"/>
       <c r="L4" s="94"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="94"/>
       <c r="B5" s="100" t="s">
         <v>91</v>
@@ -3156,7 +3009,7 @@
       <c r="K5" s="94"/>
       <c r="L5" s="94"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="94"/>
       <c r="B6" s="94"/>
       <c r="C6" s="94"/>
@@ -3170,7 +3023,7 @@
       <c r="K6" s="94"/>
       <c r="L6" s="94"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="94"/>
       <c r="B7" s="94"/>
       <c r="C7" s="94"/>
@@ -3184,7 +3037,7 @@
       <c r="K7" s="94"/>
       <c r="L7" s="94"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="94"/>
       <c r="B8" s="94"/>
       <c r="C8" s="94"/>
@@ -3198,7 +3051,7 @@
       <c r="K8" s="94"/>
       <c r="L8" s="94"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="94"/>
       <c r="B9" s="103" t="s">
         <v>94</v>
@@ -3220,7 +3073,7 @@
       <c r="K9" s="94"/>
       <c r="L9" s="94"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="94"/>
       <c r="B10" s="103" t="s">
         <v>97</v>
@@ -3238,7 +3091,7 @@
       <c r="K10" s="94"/>
       <c r="L10" s="94"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="94"/>
       <c r="B11" s="94"/>
       <c r="C11" s="94"/>
@@ -3252,7 +3105,7 @@
       <c r="K11" s="94"/>
       <c r="L11" s="94"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="94"/>
       <c r="B12" s="107" t="s">
         <v>99</v>
@@ -3268,7 +3121,7 @@
       <c r="K12" s="94"/>
       <c r="L12" s="94"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="94"/>
       <c r="B13" s="105"/>
       <c r="C13" s="104"/>
@@ -3282,7 +3135,7 @@
       <c r="K13" s="94"/>
       <c r="L13" s="94"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="94"/>
       <c r="B14" s="95"/>
       <c r="C14" s="95"/>
@@ -3296,7 +3149,7 @@
       <c r="K14" s="94"/>
       <c r="L14" s="94"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="94"/>
       <c r="B15" s="108" t="s">
         <v>100</v>
@@ -3312,7 +3165,7 @@
       <c r="K15" s="94"/>
       <c r="L15" s="94"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="94"/>
       <c r="B16" s="110" t="s">
         <v>101</v>
@@ -3328,7 +3181,7 @@
       <c r="K16" s="94"/>
       <c r="L16" s="94"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="94"/>
       <c r="B17" s="95"/>
       <c r="C17" s="95"/>
@@ -3342,7 +3195,7 @@
       <c r="K17" s="94"/>
       <c r="L17" s="94"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="94"/>
       <c r="B18" s="95"/>
       <c r="C18" s="95"/>
@@ -3356,7 +3209,7 @@
       <c r="K18" s="94"/>
       <c r="L18" s="94"/>
     </row>
-    <row r="19" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="112" t="s">
         <v>102</v>
       </c>
@@ -3384,7 +3237,7 @@
       <c r="K19" s="94"/>
       <c r="L19" s="94"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="94"/>
       <c r="B20" s="98"/>
       <c r="C20" s="95"/>
@@ -3398,7 +3251,7 @@
       <c r="K20" s="94"/>
       <c r="L20" s="94"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="94"/>
       <c r="B21" s="106"/>
       <c r="C21" s="96"/>
@@ -3412,7 +3265,7 @@
       <c r="K21" s="94"/>
       <c r="L21" s="94"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="94"/>
       <c r="B22" s="94"/>
       <c r="C22" s="94"/>
@@ -3426,7 +3279,7 @@
       <c r="K22" s="94"/>
       <c r="L22" s="94"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="94"/>
       <c r="B23" s="117" t="s">
         <v>106</v>
@@ -3452,7 +3305,7 @@
       <c r="K23" s="94"/>
       <c r="L23" s="94"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="94"/>
       <c r="B24" s="117" t="s">
         <v>106</v>
@@ -3478,7 +3331,7 @@
       <c r="K24" s="94"/>
       <c r="L24" s="94"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="94"/>
       <c r="B25" s="117" t="s">
         <v>106</v>
@@ -3504,7 +3357,7 @@
       <c r="K25" s="94"/>
       <c r="L25" s="94"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="94"/>
       <c r="B26" s="94"/>
       <c r="C26" s="94"/>
@@ -3518,7 +3371,7 @@
       <c r="K26" s="94"/>
       <c r="L26" s="94"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="94"/>
       <c r="B27" s="94"/>
       <c r="C27" s="94"/>
@@ -3532,7 +3385,7 @@
       <c r="K27" s="94"/>
       <c r="L27" s="94"/>
     </row>
-    <row r="28" spans="1:12" ht="21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="21">
       <c r="A28" s="90" t="s">
         <v>108</v>
       </c>
@@ -3552,7 +3405,7 @@
       <c r="K28" s="94"/>
       <c r="L28" s="94"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="94"/>
       <c r="B29" s="94"/>
       <c r="C29" s="94"/>
@@ -3566,7 +3419,7 @@
       <c r="K29" s="94"/>
       <c r="L29" s="94"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="94"/>
       <c r="B30" s="94"/>
       <c r="C30" s="94"/>
@@ -3580,7 +3433,7 @@
       <c r="K30" s="94"/>
       <c r="L30" s="94"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="94"/>
       <c r="B31" s="150" t="s">
         <v>111</v>
@@ -3598,7 +3451,7 @@
       <c r="K31" s="94"/>
       <c r="L31" s="94"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="94"/>
       <c r="B32" s="151"/>
       <c r="C32" s="155"/>
@@ -3612,7 +3465,7 @@
       <c r="K32" s="94"/>
       <c r="L32" s="94"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="94"/>
       <c r="B33" s="152"/>
       <c r="C33" s="157"/>
@@ -3633,20 +3486,19 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="C31:D33"/>
   </mergeCells>
-  <phoneticPr fontId="57" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -3656,7 +3508,7 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="21">
       <c r="A1" s="79" t="s">
         <v>113</v>
       </c>
@@ -3679,7 +3531,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="81"/>
       <c r="B2" s="119">
         <v>1234.56</v>
@@ -3700,7 +3552,7 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="81"/>
       <c r="B3" s="80" t="s">
         <v>118</v>
@@ -3717,7 +3569,7 @@
       <c r="F3" s="81"/>
       <c r="G3" s="81"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="81"/>
       <c r="B4" s="125">
         <v>0.48</v>
@@ -3735,22 +3587,21 @@
       <c r="G4" s="81"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="57" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="159" t="s">
         <v>122</v>
       </c>
@@ -3759,7 +3610,7 @@
       <c r="D1" s="159"/>
       <c r="E1" s="159"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="129" t="s">
         <v>123</v>
       </c>
@@ -3773,27 +3624,26 @@
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <phoneticPr fontId="57" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="23.25">
       <c r="A1" s="131" t="s">
         <v>137</v>
       </c>
@@ -3801,7 +3651,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="49.5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="46.5">
       <c r="A2" s="135" t="s">
         <v>133</v>
       </c>
@@ -3809,7 +3659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="65.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="61.5">
       <c r="A3" s="135" t="s">
         <v>136</v>
       </c>
@@ -3829,7 +3679,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="49.5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="46.5">
       <c r="A4" s="135" t="s">
         <v>131</v>
       </c>
@@ -3841,7 +3691,7 @@
         <v>41640</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="65.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="46.5">
       <c r="A5" s="135" t="s">
         <v>134</v>
       </c>
@@ -3849,7 +3699,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="49.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="46.5">
       <c r="A6" s="135" t="s">
         <v>135</v>
       </c>
@@ -3857,7 +3707,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="33.75" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="31.5">
       <c r="A7" s="135" t="s">
         <v>140</v>
       </c>
@@ -3865,7 +3715,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="23.25">
       <c r="A8" s="135" t="s">
         <v>141</v>
       </c>
@@ -3881,7 +3731,6 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <phoneticPr fontId="57" type="noConversion"/>
   <dataValidations count="7">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sorry" error="1 - 10" promptTitle="Notice" prompt="valid between 1 to 10" sqref="B2">
       <formula1>1</formula1>

</xml_diff>